<commit_message>
Remove some open questions from perf spreadsheet
</commit_message>
<xml_diff>
--- a/doc/dynalint-performance.xlsx
+++ b/doc/dynalint-performance.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
   <si>
     <t>Performance tests on my slightly modified version of Dynalint 0.1.3, which can be checked out an installed locally on your machine as follows:</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Number of Dynalint warnings</t>
   </si>
   <si>
-    <t>Why are number of warnings different?</t>
-  </si>
-  <si>
     <t>Ran 424 tests containing 660 assertions.'</t>
   </si>
   <si>
@@ -198,13 +195,13 @@
     <t>no-fn-wrapping branch of 0.1.3-jafingerhut-mods</t>
   </si>
   <si>
-    <t>TBD: NO warning on clojure.core/dissoc, which occurs 1 time pretty consistently with original dynalint.  Why?</t>
-  </si>
-  <si>
     <t>remove-most-varargs branch of 0.1.4-SNAPSHOT</t>
   </si>
   <si>
     <t>dynalint remove-most-varargs branch means this commit on that branch: 57735fb0f727eb5423b47e2bddd9b9990186edfa</t>
+  </si>
+  <si>
+    <t>NOTE: Number of warnings varies from one run to the next due to 1 second minimum interval before dynalint prints the next warning after a previous one.</t>
   </si>
 </sst>
 </file>
@@ -352,7 +349,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -360,6 +357,7 @@
     <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -764,7 +762,7 @@
   <dimension ref="A1:J110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -812,7 +810,7 @@
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:1">
@@ -857,47 +855,47 @@
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1096,7 +1094,7 @@
         <v>18</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -1116,7 +1114,7 @@
         <v>21</v>
       </c>
       <c r="I59" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -1136,7 +1134,7 @@
         <v>20</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -1181,7 +1179,7 @@
         <v>27</v>
       </c>
       <c r="C64" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D64">
         <v>37.683</v>
@@ -1196,12 +1194,7 @@
         <f>7+3</f>
         <v>10</v>
       </c>
-      <c r="I64" t="s">
-        <v>59</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="J64" s="7"/>
     </row>
     <row r="65" spans="1:10">
       <c r="D65">
@@ -1218,9 +1211,6 @@
         <f>8+2</f>
         <v>10</v>
       </c>
-      <c r="J65" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="66" spans="1:10">
       <c r="D66">
@@ -1237,9 +1227,7 @@
         <f>8+2</f>
         <v>10</v>
       </c>
-      <c r="J66" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="J66" s="2"/>
     </row>
     <row r="67" spans="1:10">
       <c r="D67">
@@ -1310,7 +1298,7 @@
         <v>27</v>
       </c>
       <c r="C72" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D72">
         <v>45.875999999999998</v>
@@ -1326,12 +1314,7 @@
         <f>7+3</f>
         <v>10</v>
       </c>
-      <c r="I72" t="s">
-        <v>59</v>
-      </c>
-      <c r="J72" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="J72" s="7"/>
     </row>
     <row r="73" spans="1:10">
       <c r="D73">
@@ -1348,9 +1331,6 @@
         <f>8+2</f>
         <v>10</v>
       </c>
-      <c r="J73" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="74" spans="1:10">
       <c r="D74">
@@ -1367,9 +1347,7 @@
         <f>8+2</f>
         <v>10</v>
       </c>
-      <c r="J74" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="J74" s="2"/>
     </row>
     <row r="75" spans="1:10">
       <c r="C75" t="s">
@@ -1411,7 +1389,7 @@
         <v>24</v>
       </c>
       <c r="B78" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C78" t="s">
         <v>29</v>
@@ -1427,7 +1405,7 @@
         <v>1.359</v>
       </c>
       <c r="I78" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -1441,7 +1419,7 @@
         <v>1.2989999999999999</v>
       </c>
       <c r="I79" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -1477,7 +1455,7 @@
         <v>24</v>
       </c>
       <c r="B83" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C83" t="s">
         <v>35</v>
@@ -1568,10 +1546,10 @@
         <v>24</v>
       </c>
       <c r="B89" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C89" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D89">
         <f>4*60+4.793</f>
@@ -1660,10 +1638,10 @@
         <v>24</v>
       </c>
       <c r="B95" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C95" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D95">
         <f>3*60+5.674</f>
@@ -1753,7 +1731,7 @@
         <v>24</v>
       </c>
       <c r="B101" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C101" t="s">
         <v>29</v>
@@ -1768,7 +1746,7 @@
         <v>0.52100000000000002</v>
       </c>
       <c r="I101" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -1815,7 +1793,7 @@
         <v>24</v>
       </c>
       <c r="B106" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C106" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Add checks for clojure.core/partition and partition-all
</commit_message>
<xml_diff>
--- a/doc/dynalint-performance.xlsx
+++ b/doc/dynalint-performance.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
   <si>
     <t>Performance tests on my slightly modified version of Dynalint 0.1.3, which can be checked out an installed locally on your machine as follows:</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>NOTE: Number of warnings varies from one run to the next due to 1 second minimum interval before dynalint prints the next warning after a previous one.</t>
+  </si>
+  <si>
+    <t>remove-most-varargs v2 branch of 0.1.4-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -276,8 +279,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -359,7 +372,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -395,6 +408,11 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -430,6 +448,11 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -759,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J72" sqref="J72"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1190,10 +1213,6 @@
       <c r="F64">
         <v>1.462</v>
       </c>
-      <c r="H64">
-        <f>7+3</f>
-        <v>10</v>
-      </c>
       <c r="J64" s="7"/>
     </row>
     <row r="65" spans="1:10">
@@ -1207,10 +1226,6 @@
       <c r="F65">
         <v>1.546</v>
       </c>
-      <c r="H65">
-        <f>8+2</f>
-        <v>10</v>
-      </c>
     </row>
     <row r="66" spans="1:10">
       <c r="D66">
@@ -1222,10 +1237,6 @@
       </c>
       <c r="F66">
         <v>1.5669999999999999</v>
-      </c>
-      <c r="H66">
-        <f>8+2</f>
-        <v>10</v>
       </c>
       <c r="J66" s="2"/>
     </row>
@@ -1298,578 +1309,778 @@
         <v>27</v>
       </c>
       <c r="C72" t="s">
+        <v>61</v>
+      </c>
+      <c r="D72">
+        <v>47.872999999999998</v>
+      </c>
+      <c r="E72">
+        <f>1*60+5.672</f>
+        <v>65.671999999999997</v>
+      </c>
+      <c r="F72">
+        <v>1.448</v>
+      </c>
+      <c r="J72" s="7"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="D73">
+        <f>1*60+2.117</f>
+        <v>62.116999999999997</v>
+      </c>
+      <c r="E73">
+        <f>1*60+20.836</f>
+        <v>80.835999999999999</v>
+      </c>
+      <c r="F73">
+        <v>1.5529999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="D74">
+        <v>57.841000000000001</v>
+      </c>
+      <c r="E74">
+        <f>1*60+15.576</f>
+        <v>75.575999999999993</v>
+      </c>
+      <c r="F74">
+        <v>1.5009999999999999</v>
+      </c>
+      <c r="J74" s="2"/>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="D75">
+        <v>47.146000000000001</v>
+      </c>
+      <c r="E75">
+        <f>1*60+4.08</f>
+        <v>64.08</v>
+      </c>
+      <c r="F75">
+        <v>1.4710000000000001</v>
+      </c>
+      <c r="J75" s="2"/>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="D76">
+        <v>50.6</v>
+      </c>
+      <c r="E76">
+        <f>1*60+8.753</f>
+        <v>68.753</v>
+      </c>
+      <c r="F76">
+        <v>1.4570000000000001</v>
+      </c>
+      <c r="J76" s="2"/>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="C77" t="s">
+        <v>36</v>
+      </c>
+      <c r="D77">
+        <f>MEDIAN(D72:D76)</f>
+        <v>50.6</v>
+      </c>
+      <c r="E77">
+        <f>MEDIAN(E72:E76)</f>
+        <v>68.753</v>
+      </c>
+      <c r="F77">
+        <f>MEDIAN(F72:F76)</f>
+        <v>1.4710000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="C78" t="s">
+        <v>39</v>
+      </c>
+      <c r="D78" s="5">
+        <f>D77/D56</f>
+        <v>3.1495082783517989</v>
+      </c>
+      <c r="E78" s="5">
+        <f>E77/E56</f>
+        <v>2.452136386332834</v>
+      </c>
+      <c r="F78" s="5">
+        <f>F77/F56</f>
+        <v>1.0620938628158845</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" t="s">
+        <v>27</v>
+      </c>
+      <c r="C80" t="s">
         <v>57</v>
       </c>
-      <c r="D72">
+      <c r="D80">
         <v>45.875999999999998</v>
       </c>
-      <c r="E72">
+      <c r="E80">
         <f>1*60+0.815</f>
         <v>60.814999999999998</v>
       </c>
-      <c r="F72">
+      <c r="F80">
         <v>1.488</v>
       </c>
-      <c r="H72">
+      <c r="H80">
         <f>7+3</f>
         <v>10</v>
       </c>
-      <c r="J72" s="7"/>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="D73">
+      <c r="J80" s="7"/>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="D81">
         <v>48.045000000000002</v>
       </c>
-      <c r="E73">
+      <c r="E81">
         <f>1*60+2.774</f>
         <v>62.774000000000001</v>
       </c>
-      <c r="F73">
+      <c r="F81">
         <v>1.4930000000000001</v>
       </c>
-      <c r="H73">
+      <c r="H81">
         <f>8+2</f>
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
-      <c r="D74">
+    <row r="82" spans="1:10">
+      <c r="D82">
         <v>46.595999999999997</v>
       </c>
-      <c r="E74">
+      <c r="E82">
         <f>1*60+1.5</f>
         <v>61.5</v>
       </c>
-      <c r="F74">
+      <c r="F82">
         <v>1.4830000000000001</v>
       </c>
-      <c r="H74">
+      <c r="H82">
         <f>8+2</f>
         <v>10</v>
       </c>
-      <c r="J74" s="2"/>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="C75" t="s">
+      <c r="J82" s="2"/>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="C83" t="s">
         <v>36</v>
       </c>
-      <c r="D75">
-        <f>MEDIAN(D72:D74)</f>
+      <c r="D83">
+        <f>MEDIAN(D80:D82)</f>
         <v>46.595999999999997</v>
       </c>
-      <c r="E75">
-        <f>MEDIAN(E72:E74)</f>
+      <c r="E83">
+        <f>MEDIAN(E80:E82)</f>
         <v>61.5</v>
       </c>
-      <c r="F75">
-        <f>MEDIAN(F72:F74)</f>
+      <c r="F83">
+        <f>MEDIAN(F80:F82)</f>
         <v>1.488</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
-      <c r="C76" t="s">
+    <row r="84" spans="1:10">
+      <c r="C84" t="s">
         <v>39</v>
       </c>
-      <c r="D76" s="5">
-        <f>D75/D56</f>
+      <c r="D84" s="5">
+        <f>D83/D56</f>
         <v>2.9002863189343957</v>
       </c>
-      <c r="E76" s="5">
-        <f>E75/E56</f>
+      <c r="E84" s="5">
+        <f>E83/E56</f>
         <v>2.1934517440616306</v>
       </c>
-      <c r="F76" s="5">
-        <f>F75/F56</f>
+      <c r="F84" s="5">
+        <f>F83/F56</f>
         <v>1.0743682310469314</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="6" customFormat="1"/>
-    <row r="78" spans="1:10">
-      <c r="A78" t="s">
+    <row r="85" spans="1:10" s="6" customFormat="1"/>
+    <row r="86" spans="1:10">
+      <c r="A86" t="s">
         <v>24</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B86" t="s">
         <v>46</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C86" t="s">
         <v>29</v>
       </c>
-      <c r="D78">
+      <c r="D86">
         <f>42.973</f>
         <v>42.972999999999999</v>
       </c>
-      <c r="E78">
+      <c r="E86">
         <v>50.735999999999997</v>
       </c>
-      <c r="F78">
+      <c r="F86">
         <v>1.359</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I86" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
-      <c r="D79">
+    <row r="87" spans="1:10">
+      <c r="D87">
         <v>43.085999999999999</v>
       </c>
-      <c r="E79">
+      <c r="E87">
         <v>51.256999999999998</v>
       </c>
-      <c r="F79">
+      <c r="F87">
         <v>1.2989999999999999</v>
       </c>
-      <c r="I79" t="s">
+      <c r="I87" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
-      <c r="D80">
+    <row r="88" spans="1:10">
+      <c r="D88">
         <v>42.835000000000001</v>
       </c>
-      <c r="E80">
+      <c r="E88">
         <v>51.097999999999999</v>
       </c>
-      <c r="F80">
+      <c r="F88">
         <v>1.302</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
-      <c r="C81" t="s">
+    <row r="89" spans="1:10">
+      <c r="C89" t="s">
         <v>36</v>
       </c>
-      <c r="D81" s="3">
-        <f>MEDIAN(D78:D80)</f>
+      <c r="D89" s="3">
+        <f>MEDIAN(D86:D88)</f>
         <v>42.972999999999999</v>
       </c>
-      <c r="E81" s="3">
-        <f>MEDIAN(E78:E80)</f>
+      <c r="E89" s="3">
+        <f>MEDIAN(E86:E88)</f>
         <v>51.097999999999999</v>
       </c>
-      <c r="F81" s="3">
-        <f>MEDIAN(F78:F80)</f>
+      <c r="F89" s="3">
+        <f>MEDIAN(F86:F88)</f>
         <v>1.302</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
-      <c r="A83" t="s">
+    <row r="91" spans="1:10">
+      <c r="A91" t="s">
         <v>24</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B91" t="s">
         <v>46</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C91" t="s">
         <v>35</v>
       </c>
-      <c r="D83">
+      <c r="D91">
         <f>9*60+36.333</f>
         <v>576.33299999999997</v>
       </c>
-      <c r="E83">
+      <c r="E91">
         <f>9*60+56.853</f>
         <v>596.85299999999995</v>
       </c>
-      <c r="F83">
+      <c r="F91">
         <v>4.04</v>
       </c>
-      <c r="H83">
+      <c r="H91">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
-      <c r="D84">
+    <row r="92" spans="1:10">
+      <c r="D92">
         <f>9*60+17.366</f>
         <v>557.36599999999999</v>
       </c>
-      <c r="E84">
+      <c r="E92">
         <f>9*60+40.505</f>
         <v>580.505</v>
       </c>
-      <c r="F84">
+      <c r="F92">
         <v>4.234</v>
       </c>
-      <c r="H84">
+      <c r="H92">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
-      <c r="D85">
+    <row r="93" spans="1:10">
+      <c r="D93">
         <f>9*60+21.663</f>
         <v>561.66300000000001</v>
       </c>
-      <c r="E85">
+      <c r="E93">
         <f>9*60+44.215</f>
         <v>584.21500000000003</v>
       </c>
-      <c r="F85">
+      <c r="F93">
         <v>4.21</v>
       </c>
-      <c r="H85">
+      <c r="H93">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
-      <c r="C86" t="s">
+    <row r="94" spans="1:10">
+      <c r="C94" t="s">
         <v>36</v>
       </c>
-      <c r="D86">
-        <f>MEDIAN(D83:D85)</f>
+      <c r="D94">
+        <f>MEDIAN(D91:D93)</f>
         <v>561.66300000000001</v>
       </c>
-      <c r="E86">
-        <f>MEDIAN(E83:E85)</f>
+      <c r="E94">
+        <f>MEDIAN(E91:E93)</f>
         <v>584.21500000000003</v>
       </c>
-      <c r="F86">
-        <f>MEDIAN(F83:F85)</f>
+      <c r="F94">
+        <f>MEDIAN(F91:F93)</f>
         <v>4.21</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
-      <c r="C87" t="s">
+    <row r="95" spans="1:10">
+      <c r="C95" t="s">
         <v>39</v>
       </c>
-      <c r="D87" s="5">
-        <f>D86/D81</f>
+      <c r="D95" s="5">
+        <f>D94/D89</f>
         <v>13.070137062806879</v>
       </c>
-      <c r="E87" s="5">
-        <f>E86/E81</f>
+      <c r="E95" s="5">
+        <f>E94/E89</f>
         <v>11.433226349367882</v>
       </c>
-      <c r="F87" s="5">
-        <f>F86/F81</f>
+      <c r="F95" s="5">
+        <f>F94/F89</f>
         <v>3.2334869431643622</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
-      <c r="A89" t="s">
+    <row r="97" spans="1:8">
+      <c r="A97" t="s">
         <v>24</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B97" t="s">
         <v>46</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C97" t="s">
         <v>58</v>
       </c>
-      <c r="D89">
+      <c r="D97">
         <f>4*60+4.793</f>
         <v>244.79300000000001</v>
       </c>
-      <c r="E89">
+      <c r="E97">
         <f>4*60+20.897</f>
         <v>260.89699999999999</v>
       </c>
-      <c r="F89">
+      <c r="F97">
         <v>2.3290000000000002</v>
       </c>
-      <c r="H89">
+      <c r="H97">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
-      <c r="D90">
+    <row r="98" spans="1:8">
+      <c r="D98">
         <f>4*60+6.784</f>
         <v>246.78399999999999</v>
       </c>
-      <c r="E90">
+      <c r="E98">
         <f>4*60+22.296</f>
         <v>262.29599999999999</v>
       </c>
-      <c r="F90">
+      <c r="F98">
         <v>2.2669999999999999</v>
       </c>
-      <c r="H90">
+      <c r="H98">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
-      <c r="D91">
+    <row r="99" spans="1:8">
+      <c r="D99">
         <f>4*60+11.235</f>
         <v>251.23500000000001</v>
       </c>
-      <c r="E91">
+      <c r="E99">
         <f>4*60+27.694</f>
         <v>267.69400000000002</v>
       </c>
-      <c r="F91">
+      <c r="F99">
         <f>2.278</f>
         <v>2.278</v>
       </c>
-      <c r="H91">
+      <c r="H99">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
-      <c r="C92" t="s">
+    <row r="100" spans="1:8">
+      <c r="C100" t="s">
         <v>36</v>
       </c>
-      <c r="D92">
-        <f>MEDIAN(D89:D91)</f>
+      <c r="D100">
+        <f>MEDIAN(D97:D99)</f>
         <v>246.78399999999999</v>
       </c>
-      <c r="E92">
-        <f>MEDIAN(E89:E91)</f>
+      <c r="E100">
+        <f>MEDIAN(E97:E99)</f>
         <v>262.29599999999999</v>
       </c>
-      <c r="F92">
-        <f>MEDIAN(F89:F91)</f>
+      <c r="F100">
+        <f>MEDIAN(F97:F99)</f>
         <v>2.278</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
-      <c r="C93" t="s">
+    <row r="101" spans="1:8">
+      <c r="C101" t="s">
         <v>39</v>
       </c>
-      <c r="D93" s="5">
-        <f>D92/D81</f>
+      <c r="D101" s="5">
+        <f>D100/D89</f>
         <v>5.7427687152398015</v>
       </c>
-      <c r="E93" s="5">
-        <f>E92/E81</f>
+      <c r="E101" s="5">
+        <f>E100/E89</f>
         <v>5.1331950369877486</v>
       </c>
-      <c r="F93" s="5">
-        <f>F92/F81</f>
+      <c r="F101" s="5">
+        <f>F100/F89</f>
         <v>1.749615975422427</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
-      <c r="A95" t="s">
+    <row r="103" spans="1:8">
+      <c r="A103" t="s">
         <v>24</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B103" t="s">
         <v>46</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C103" t="s">
+        <v>61</v>
+      </c>
+      <c r="D103">
+        <f>4*60+30.699</f>
+        <v>270.69900000000001</v>
+      </c>
+      <c r="E103">
+        <f>4*60+47.56</f>
+        <v>287.56</v>
+      </c>
+      <c r="F103">
+        <v>2.359</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="D104">
+        <f>4*60+28.106</f>
+        <v>268.10599999999999</v>
+      </c>
+      <c r="E104">
+        <f>4*60+44.405</f>
+        <v>284.40499999999997</v>
+      </c>
+      <c r="F104">
+        <f>2.334</f>
+        <v>2.3340000000000001</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="D105">
+        <f>4*60+24.765</f>
+        <v>264.76499999999999</v>
+      </c>
+      <c r="E105">
+        <f>4*60+41.358</f>
+        <v>281.358</v>
+      </c>
+      <c r="F105">
+        <v>2.33</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="C106" t="s">
+        <v>36</v>
+      </c>
+      <c r="D106">
+        <f>MEDIAN(D103:D105)</f>
+        <v>268.10599999999999</v>
+      </c>
+      <c r="E106">
+        <f>MEDIAN(E103:E105)</f>
+        <v>284.40499999999997</v>
+      </c>
+      <c r="F106">
+        <f>MEDIAN(F103:F105)</f>
+        <v>2.3340000000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="C107" t="s">
+        <v>39</v>
+      </c>
+      <c r="D107" s="5">
+        <f>D106/D89</f>
+        <v>6.2389407302259556</v>
+      </c>
+      <c r="E107" s="5">
+        <f>E106/E89</f>
+        <v>5.5658734197033146</v>
+      </c>
+      <c r="F107" s="5">
+        <f>F106/F89</f>
+        <v>1.792626728110599</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109" t="s">
+        <v>24</v>
+      </c>
+      <c r="B109" t="s">
+        <v>46</v>
+      </c>
+      <c r="C109" t="s">
         <v>57</v>
       </c>
-      <c r="D95">
+      <c r="D109">
         <f>3*60+5.674</f>
         <v>185.67400000000001</v>
       </c>
-      <c r="E95">
+      <c r="E109">
         <f>3*60+19.55</f>
         <v>199.55</v>
       </c>
-      <c r="F95">
+      <c r="F109">
         <f>2.06</f>
         <v>2.06</v>
       </c>
-      <c r="H95">
+      <c r="H109">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
-      <c r="D96">
+    <row r="110" spans="1:8">
+      <c r="D110">
         <f>3*60+2.687</f>
         <v>182.68700000000001</v>
       </c>
-      <c r="E96">
+      <c r="E110">
         <f>3*60+16.613</f>
         <v>196.613</v>
       </c>
-      <c r="F96">
+      <c r="F110">
         <v>1.9730000000000001</v>
       </c>
-      <c r="H96">
+      <c r="H110">
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
-      <c r="D97">
+    <row r="111" spans="1:8">
+      <c r="D111">
         <f>3*60+2.341</f>
         <v>182.34100000000001</v>
       </c>
-      <c r="E97">
+      <c r="E111">
         <f>3*60+17.059</f>
         <v>197.059</v>
       </c>
-      <c r="F97">
+      <c r="F111">
         <v>2.024</v>
       </c>
-      <c r="H97">
+      <c r="H111">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
-      <c r="C98" t="s">
+    <row r="112" spans="1:8">
+      <c r="C112" t="s">
         <v>36</v>
       </c>
-      <c r="D98">
-        <f>MEDIAN(D95:D97)</f>
+      <c r="D112">
+        <f>MEDIAN(D109:D111)</f>
         <v>182.68700000000001</v>
       </c>
-      <c r="E98">
-        <f>MEDIAN(E95:E97)</f>
+      <c r="E112">
+        <f>MEDIAN(E109:E111)</f>
         <v>197.059</v>
       </c>
-      <c r="F98">
-        <f>MEDIAN(F95:F97)</f>
+      <c r="F112">
+        <f>MEDIAN(F109:F111)</f>
         <v>2.024</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
-      <c r="C99" t="s">
+    <row r="113" spans="1:9">
+      <c r="C113" t="s">
         <v>39</v>
       </c>
-      <c r="D99" s="5">
-        <f>D98/D81</f>
+      <c r="D113" s="5">
+        <f>D112/D89</f>
         <v>4.2512042445256331</v>
       </c>
-      <c r="E99" s="5">
-        <f>E98/E81</f>
+      <c r="E113" s="5">
+        <f>E112/E89</f>
         <v>3.8564914478061763</v>
       </c>
-      <c r="F99" s="5">
-        <f>F98/F81</f>
+      <c r="F113" s="5">
+        <f>F112/F89</f>
         <v>1.5545314900153608</v>
       </c>
     </row>
-    <row r="100" spans="1:9" s="6" customFormat="1"/>
-    <row r="101" spans="1:9">
-      <c r="A101" t="s">
+    <row r="114" spans="1:9" s="6" customFormat="1"/>
+    <row r="115" spans="1:9">
+      <c r="A115" t="s">
         <v>24</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B115" t="s">
         <v>55</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C115" t="s">
         <v>29</v>
       </c>
-      <c r="D101">
+      <c r="D115">
         <v>5.2480000000000002</v>
       </c>
-      <c r="E101">
+      <c r="E115">
         <v>5.9089999999999998</v>
       </c>
-      <c r="F101">
+      <c r="F115">
         <v>0.52100000000000002</v>
       </c>
-      <c r="I101" t="s">
+      <c r="I115" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
-      <c r="D102">
+    <row r="116" spans="1:9">
+      <c r="D116">
         <v>5.2469999999999999</v>
       </c>
-      <c r="E102">
+      <c r="E116">
         <v>5.8860000000000001</v>
       </c>
-      <c r="F102">
+      <c r="F116">
         <v>0.51500000000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
-      <c r="D103">
+    <row r="117" spans="1:9">
+      <c r="D117">
         <v>5.3520000000000003</v>
       </c>
-      <c r="E103">
+      <c r="E117">
         <v>6.0110000000000001</v>
       </c>
-      <c r="F103">
+      <c r="F117">
         <v>0.53100000000000003</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
-      <c r="C104" t="s">
+    <row r="118" spans="1:9">
+      <c r="C118" t="s">
         <v>36</v>
       </c>
-      <c r="D104" s="3">
-        <f>MEDIAN(D101:D103)</f>
+      <c r="D118" s="3">
+        <f>MEDIAN(D115:D117)</f>
         <v>5.2480000000000002</v>
       </c>
-      <c r="E104" s="3">
-        <f>MEDIAN(E101:E103)</f>
+      <c r="E118" s="3">
+        <f>MEDIAN(E115:E117)</f>
         <v>5.9089999999999998</v>
       </c>
-      <c r="F104" s="3">
-        <f>MEDIAN(F101:F103)</f>
+      <c r="F118" s="3">
+        <f>MEDIAN(F115:F117)</f>
         <v>0.52100000000000002</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
-      <c r="A106" t="s">
+    <row r="120" spans="1:9">
+      <c r="A120" t="s">
         <v>24</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B120" t="s">
         <v>55</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C120" t="s">
         <v>35</v>
       </c>
-      <c r="D106">
+      <c r="D120">
         <v>10.487</v>
       </c>
-      <c r="E106">
+      <c r="E120">
         <v>11.236000000000001</v>
       </c>
-      <c r="F106">
+      <c r="F120">
         <v>0.80200000000000005</v>
       </c>
-      <c r="H106">
+      <c r="H120">
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
-      <c r="D107">
+    <row r="121" spans="1:9">
+      <c r="D121">
         <v>10.071</v>
       </c>
-      <c r="E107">
+      <c r="E121">
         <v>10.737</v>
       </c>
-      <c r="F107">
+      <c r="F121">
         <v>0.76400000000000001</v>
       </c>
-      <c r="H107">
+      <c r="H121">
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
-      <c r="D108">
+    <row r="122" spans="1:9">
+      <c r="D122">
         <v>10.185</v>
       </c>
-      <c r="E108">
+      <c r="E122">
         <v>10.81</v>
       </c>
-      <c r="F108">
+      <c r="F122">
         <v>0.79300000000000004</v>
       </c>
-      <c r="H108">
+      <c r="H122">
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
-      <c r="C109" t="s">
+    <row r="123" spans="1:9">
+      <c r="C123" t="s">
         <v>36</v>
       </c>
-      <c r="D109">
-        <f>MEDIAN(D106:D108)</f>
+      <c r="D123">
+        <f>MEDIAN(D120:D122)</f>
         <v>10.185</v>
       </c>
-      <c r="E109">
-        <f>MEDIAN(E106:E108)</f>
+      <c r="E123">
+        <f>MEDIAN(E120:E122)</f>
         <v>10.81</v>
       </c>
-      <c r="F109">
-        <f>MEDIAN(F106:F108)</f>
+      <c r="F123">
+        <f>MEDIAN(F120:F122)</f>
         <v>0.79300000000000004</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
-      <c r="C110" t="s">
+    <row r="124" spans="1:9">
+      <c r="C124" t="s">
         <v>39</v>
       </c>
-      <c r="D110" s="5">
-        <f>D109/D104</f>
+      <c r="D124" s="5">
+        <f>D123/D118</f>
         <v>1.9407393292682926</v>
       </c>
-      <c r="E110" s="5">
-        <f>E109/E104</f>
+      <c r="E124" s="5">
+        <f>E123/E118</f>
         <v>1.8294127601963108</v>
       </c>
-      <c r="F110" s="5">
-        <f>F109/F104</f>
+      <c r="F124" s="5">
+        <f>F123/F118</f>
         <v>1.5220729366602688</v>
       </c>
     </row>

</xml_diff>